<commit_message>
Polished ClimbWinchCmd & general cleanup of command constructors
</commit_message>
<xml_diff>
--- a/Joystick Mapping.xlsx
+++ b/Joystick Mapping.xlsx
@@ -39,34 +39,16 @@
     <t xml:space="preserve">Control panel Spinner</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Control panel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Unfold</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Climb Release</t>
+    <t xml:space="preserve">Control panel Unfold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climb Winch Down</t>
   </si>
   <si>
     <t xml:space="preserve">Intake</t>
   </si>
   <si>
-    <t xml:space="preserve">Climb Winch</t>
+    <t xml:space="preserve">Climb Winch Up</t>
   </si>
   <si>
     <t xml:space="preserve">Kill Everything</t>
@@ -97,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -148,12 +130,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -212,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,10 +237,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,11 +249,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,9 +284,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1208160</xdr:colOff>
+      <xdr:colOff>1207800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -328,8 +300,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4360680" y="697320"/>
-          <a:ext cx="5978520" cy="3157560"/>
+          <a:off x="4361400" y="697320"/>
+          <a:ext cx="5978160" cy="3157200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -350,9 +322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1255680</xdr:colOff>
+      <xdr:colOff>1255320</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>221400</xdr:rowOff>
+      <xdr:rowOff>221040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -366,8 +338,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4408200" y="5842080"/>
-          <a:ext cx="5978520" cy="3016440"/>
+          <a:off x="4408920" y="5842080"/>
+          <a:ext cx="5978160" cy="3016080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -389,8 +361,8 @@
   </sheetPr>
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -451,7 +423,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="8"/>
@@ -462,7 +434,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="8"/>
@@ -484,7 +456,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -494,10 +466,10 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
@@ -533,8 +505,8 @@
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0"/>
@@ -542,8 +514,8 @@
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0"/>
@@ -551,8 +523,8 @@
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0"/>
@@ -560,8 +532,8 @@
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0"/>
@@ -569,8 +541,8 @@
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="0"/>
@@ -674,7 +646,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -692,7 +664,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-      <c r="H35" s="18"/>
+      <c r="H35" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>